<commit_message>
Update annual reporting summary table.
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_ldn_annual.xlsx
+++ b/LDMP/data/summary_table_ldn_annual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C404BEBB-51D9-4F0F-9B94-1AF651996B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1336C9-3779-402A-AE8A-D599ABCFD0A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1707,11 +1707,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2241,12 +2242,15 @@
     <mergeCell ref="A17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="63" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4326,12 +4330,15 @@
     <mergeCell ref="B76:B82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="57" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -4886,12 +4893,15 @@
     <mergeCell ref="A27:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5479,6 +5489,6 @@
     <mergeCell ref="A26:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>